<commit_message>
slices results and code
</commit_message>
<xml_diff>
--- a/results/spreadsheets/Results - Burgers Viscosity.xlsx
+++ b/results/spreadsheets/Results - Burgers Viscosity.xlsx
@@ -120,9 +120,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000E+00"/>
     <numFmt numFmtId="165" formatCode="0.000%"/>
+    <numFmt numFmtId="166" formatCode="0.0000%"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -361,7 +362,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -424,6 +425,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -16231,10 +16233,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N359"/>
+  <dimension ref="A1:S359"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24:I43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S17" sqref="Q17:S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16243,6 +16245,7 @@
     <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.42578125" customWidth="1"/>
+    <col min="18" max="19" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -16271,7 +16274,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="20"/>
       <c r="B2" s="22"/>
       <c r="C2" s="2" t="s">
@@ -16925,7 +16928,7 @@
         <v>0.41731643207999602</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -16968,8 +16971,9 @@
         <f>AVERAGE($L17:L17)</f>
         <v>0.26540259939308702</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="S17" s="30"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -17013,7 +17017,7 @@
         <v>0.31681425570123101</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -17057,7 +17061,7 @@
         <v>0.26257686856658202</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -17101,7 +17105,7 @@
         <v>0.397195846064686</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -17145,7 +17149,7 @@
         <v>0.52465425773965702</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -17189,7 +17193,7 @@
         <v>0.84554490648357505</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="14"/>
       <c r="B23" s="14"/>
       <c r="C23" s="14"/>
@@ -17217,7 +17221,7 @@
       </c>
       <c r="N23" s="14"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -17261,7 +17265,7 @@
         <v>0.46130444884000499</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -17305,7 +17309,7 @@
         <v>1.52334351684767E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -17349,7 +17353,7 @@
         <v>0.65169257607410702</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>20</v>
       </c>
@@ -17393,7 +17397,7 @@
         <v>0.58471573638440399</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>20</v>
       </c>
@@ -17437,7 +17441,7 @@
         <v>0.66468092130704004</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>20</v>
       </c>
@@ -17481,7 +17485,7 @@
         <v>0.52337340219818196</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>20</v>
       </c>
@@ -17525,7 +17529,7 @@
         <v>0.55705301540155905</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>20</v>
       </c>
@@ -17569,7 +17573,7 @@
         <v>0.18424698047267099</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>20</v>
       </c>
@@ -31754,6 +31758,7 @@
     <mergeCell ref="M1:M2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -31781,8 +31786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N359"/>
   <sheetViews>
-    <sheetView topLeftCell="A339" workbookViewId="0">
-      <selection activeCell="D355" sqref="D355"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>